<commit_message>
Implemented drive search, improved UI, swallow exceptions in JAudioTags.
</commit_message>
<xml_diff>
--- a/_Docs, stuff/ID3 tag comparison.xlsx
+++ b/_Docs, stuff/ID3 tag comparison.xlsx
@@ -105,14 +105,6 @@
     <t>- nuGet package</t>
   </si>
   <si>
-    <t>- last update few weeks ago</t>
-  </si>
-  <si>
-    <t>- poor documentation
-- lack of examples
-- might be overkill for audio purposes</t>
-  </si>
-  <si>
     <t>- easiest usage
 - good documentation
 - proper format handling, not overkill</t>
@@ -127,6 +119,15 @@
   </si>
   <si>
     <t>- handles ID3 versions: v1, v2.3, v2.4</t>
+  </si>
+  <si>
+    <t>- poor documentation
+- lack of examplex</t>
+  </si>
+  <si>
+    <t>- last update few weeks ago
+- nuGet package
+- handles ID3 versions: v1, v2.3, v2.4</t>
   </si>
 </sst>
 </file>
@@ -170,7 +171,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,12 +184,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -487,19 +482,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,7 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
@@ -831,11 +828,11 @@
       <c r="C2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>28</v>
+      <c r="D2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>17</v>
@@ -868,7 +865,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -877,11 +874,11 @@
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>29</v>
+      <c r="D4" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>16</v>
@@ -900,11 +897,11 @@
       <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>31</v>
+      <c r="D5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>10</v>

</xml_diff>